<commit_message>
update - ProductVariation - add quantity alert
</commit_message>
<xml_diff>
--- a/core/seed_products_productvariation.xlsx
+++ b/core/seed_products_productvariation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420BE9F5-6167-4A97-8ECB-AC58983ABF3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C44DF2D-2B6A-4C76-AC57-158F90E86661}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>NAME</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>CONSUMABLE</t>
+  </si>
+  <si>
+    <t>QUANTITY ALERT</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1049,7 +1052,7 @@
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1074,8 +1077,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1091,8 +1097,11 @@
       <c r="G2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1108,8 +1117,11 @@
       <c r="G3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1142,8 +1154,11 @@
       <c r="G5">
         <v>150</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1159,8 +1174,11 @@
       <c r="G6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1176,8 +1194,11 @@
       <c r="G7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1193,8 +1214,11 @@
       <c r="G8">
         <v>150</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1210,8 +1234,11 @@
       <c r="G9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1224,8 +1251,11 @@
       <c r="F10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1241,8 +1271,11 @@
       <c r="G11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1258,8 +1291,11 @@
       <c r="G12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1275,8 +1311,11 @@
       <c r="G13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1292,8 +1331,11 @@
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1309,8 +1351,11 @@
       <c r="G15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1326,8 +1371,11 @@
       <c r="G16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1343,8 +1391,11 @@
       <c r="G17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1360,8 +1411,11 @@
       <c r="G18">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1377,8 +1431,11 @@
       <c r="G19">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1394,8 +1451,11 @@
       <c r="G20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1411,8 +1471,11 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1427,6 +1490,9 @@
       </c>
       <c r="G22">
         <v>1</v>
+      </c>
+      <c r="I22">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>